<commit_message>
Change 08 input Excel file
</commit_message>
<xml_diff>
--- a/excel-input/08-various-bounds/08-various-bounds.xlsx
+++ b/excel-input/08-various-bounds/08-various-bounds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="expert" sheetId="1" state="visible" r:id="rId3"/>
@@ -339,64 +339,64 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Alojzy</t>
+    <t xml:space="preserve">Alojzy</t>
   </si>
   <si>
     <t xml:space="preserve">1 task, no bounds</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Barłomiej</t>
+    <t xml:space="preserve">Barłomiej</t>
   </si>
   <si>
     <t xml:space="preserve">1 task, 1 xbday</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Cezary</t>
+    <t xml:space="preserve">Cezary</t>
   </si>
   <si>
     <t xml:space="preserve">1 task, 2 xbday</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Dariusz</t>
+    <t xml:space="preserve">Dariusz</t>
   </si>
   <si>
     <t xml:space="preserve">1 task</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Eugenius</t>
+    <t xml:space="preserve">Eugeniusz</t>
   </si>
   <si>
     <t xml:space="preserve">2 tasks, no bounds</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Franciszek</t>
+    <t xml:space="preserve">Franciszek</t>
   </si>
   <si>
     <t xml:space="preserve">2 tasks, 1 ubday</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Gustaw</t>
+    <t xml:space="preserve">Gustaw</t>
   </si>
   <si>
     <t xml:space="preserve">2 tasks</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Hubert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.Ignacy</t>
+    <t xml:space="preserve">Hubert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignacy</t>
   </si>
   <si>
     <t xml:space="preserve">3 tasks, no bounds</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Jarosław</t>
+    <t xml:space="preserve">Jarosław</t>
   </si>
   <si>
     <t xml:space="preserve">3 tasks, 1 ubday(2)</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.Paweł</t>
+    <t xml:space="preserve">Paweł</t>
   </si>
   <si>
     <t xml:space="preserve">3 tasks, 1 ubday(1)</t>
@@ -411,67 +411,67 @@
     <t xml:space="preserve">Work</t>
   </si>
   <si>
-    <t xml:space="preserve">DEV.p1.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p2.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p3.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p4.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p5.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p6.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p7.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p8.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p9.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p10.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p11.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p12.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p13.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p14.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p15.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p16.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p17.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p18.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p19.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p20.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEV.p21.m</t>
+    <t xml:space="preserve">t1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t21</t>
   </si>
   <si>
     <t xml:space="preserve">Expert</t>
@@ -698,7 +698,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -708,7 +708,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFD8CE"/>
-        <bgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFFFD7"/>
       </patternFill>
     </fill>
     <fill>
@@ -727,12 +727,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFD7"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD7D7"/>
-        <bgColor rgb="FFFFD8CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -776,7 +770,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -817,20 +811,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -873,15 +871,19 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -923,7 +925,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFFFD7D7"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1074,8 +1076,8 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="D1:D2 B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1248,15 +1250,16 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1:D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1272,12 +1275,12 @@
       <c r="D1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="26" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="n">
+      <c r="A2" s="17" t="n">
         <v>45641</v>
       </c>
       <c r="B2" s="5" t="n">
@@ -1289,7 +1292,7 @@
       <c r="D2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="25" t="n">
+      <c r="E2" s="27" t="n">
         <f aca="false">MAX(MAX(period!C2:C898),MAX(task!C2:C896))</f>
         <v>45795</v>
       </c>
@@ -1313,7 +1316,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="1" sqref="D1:D2 I5"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1323,7 +1326,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1341,10 +1344,10 @@
       <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="26" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1358,11 +1361,11 @@
       <c r="D2" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="E2" s="14" t="n">
+      <c r="E2" s="15" t="n">
         <f aca="false">misc!A2+1</f>
         <v>45642</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="15" t="n">
         <f aca="false">E2+20</f>
         <v>45662</v>
       </c>
@@ -1393,19 +1396,19 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="D1:D2 E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.46"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="27" width="23.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="29" width="23.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1419,10 +1422,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>75</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -1447,8 +1450,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="D1:D2 E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1458,7 +1461,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>76</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1472,10 +1475,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -1500,8 +1503,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="D1:D2 C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1511,7 +1514,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1541,8 +1544,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="D1:D2 C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1552,7 +1555,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>80</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1566,7 +1569,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="5" t="n">
@@ -1594,8 +1597,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D1:D2 B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1605,7 +1608,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>85</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1619,7 +1622,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -1647,8 +1650,8 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D1:D2 B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1660,7 +1663,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1683,10 +1686,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>75</v>
       </c>
       <c r="D2" s="5" t="n">
@@ -1721,7 +1724,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="D1:D2 B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1731,7 +1734,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1761,8 +1764,8 @@
   </sheetPr>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="D1:D2 B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2363,8 +2366,8 @@
   </sheetPr>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="D1:D2 C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2407,10 +2410,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C3" s="13" t="b">
@@ -2439,10 +2442,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="13" t="b">
@@ -2487,10 +2490,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="14" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="13" t="b">
@@ -2503,10 +2506,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="14" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="13" t="b">
@@ -2551,10 +2554,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="13" t="b">
@@ -2567,10 +2570,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="13" t="b">
@@ -2647,10 +2650,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="14" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="13" t="b">
@@ -2663,10 +2666,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C19" s="13" t="b">
@@ -2679,10 +2682,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="13" t="b">
@@ -2777,8 +2780,8 @@
   </sheetPr>
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="1" sqref="D1:D2 E5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2828,10 +2831,10 @@
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="15" t="n">
         <v>45643</v>
       </c>
-      <c r="D2" s="14" t="n">
+      <c r="D2" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="E2" s="1" t="n">
@@ -2854,22 +2857,22 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="15" t="n">
+      <c r="C3" s="16" t="n">
         <v>45644</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="16" t="n">
         <v>45646</v>
       </c>
-      <c r="E3" s="10" t="n">
+      <c r="E3" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F3" s="14" t="n">
         <v>5</v>
       </c>
       <c r="G3" s="13" t="b">
@@ -2886,22 +2889,22 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="15" t="n">
+      <c r="C4" s="16" t="n">
         <v>45649</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="16" t="n">
         <v>45653</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F4" s="14" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="13" t="b">
@@ -3314,8 +3317,8 @@
   </sheetPr>
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3354,10 +3357,10 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="14" t="n">
+      <c r="B2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -3376,19 +3379,19 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14" t="n">
+      <c r="B3" s="16" t="n">
         <v>45642</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C3" s="16" t="n">
         <v>45653</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="n">
+      <c r="D3" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="b">
@@ -3404,10 +3407,10 @@
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="14" t="n">
+      <c r="B4" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="C4" s="14" t="n">
+      <c r="C4" s="15" t="n">
         <v>45653</v>
       </c>
       <c r="D4" s="1" t="n">
@@ -3426,19 +3429,19 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="14" t="n">
+      <c r="B5" s="16" t="n">
         <v>45642</v>
       </c>
-      <c r="C5" s="14" t="n">
+      <c r="C5" s="16" t="n">
         <v>45653</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="n">
+      <c r="D5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="b">
@@ -3451,20 +3454,20 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
@@ -3859,8 +3862,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="D1:D2 G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3899,10 +3902,10 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="14" t="n">
+      <c r="B2" s="15" t="n">
         <v>45642</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="15" t="n">
         <v>45689</v>
       </c>
       <c r="D2" s="5" t="n">
@@ -3924,10 +3927,10 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="n">
+      <c r="B3" s="15" t="n">
         <v>45690</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C3" s="15" t="n">
         <v>45717</v>
       </c>
       <c r="D3" s="5" t="n">
@@ -3946,148 +3949,148 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4108,14 +4111,14 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="D1:D2 C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="16" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="17" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.53"/>
   </cols>
   <sheetData>
@@ -4123,10 +4126,10 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="9" t="b">
@@ -4135,13 +4138,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="19" t="n">
+      <c r="B2" s="20" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="19" t="n">
+      <c r="C2" s="20" t="n">
         <v>45672</v>
       </c>
       <c r="D2" s="2" t="b">
@@ -4150,13 +4153,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="19" t="n">
+      <c r="B3" s="20" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="19" t="n">
+      <c r="C3" s="20" t="n">
         <v>45701</v>
       </c>
       <c r="D3" s="2" t="b">
@@ -4165,13 +4168,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="19" t="n">
+      <c r="B4" s="20" t="n">
         <v>45702</v>
       </c>
-      <c r="C4" s="19" t="n">
+      <c r="C4" s="20" t="n">
         <v>45732</v>
       </c>
       <c r="D4" s="2" t="b">
@@ -4180,13 +4183,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="19" t="n">
+      <c r="B5" s="20" t="n">
         <v>45733</v>
       </c>
-      <c r="C5" s="19" t="n">
+      <c r="C5" s="20" t="n">
         <v>45761</v>
       </c>
       <c r="D5" s="2" t="b">
@@ -4195,13 +4198,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="19" t="n">
+      <c r="B6" s="20" t="n">
         <v>45762</v>
       </c>
-      <c r="C6" s="19" t="n">
+      <c r="C6" s="20" t="n">
         <v>45795</v>
       </c>
       <c r="D6" s="2" t="b">
@@ -4210,8 +4213,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4232,14 +4235,14 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="1" sqref="D1:D2 H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="21" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="5" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.53"/>
   </cols>
@@ -4267,16 +4270,16 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="22" t="n">
+      <c r="C2" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="22" t="n">
+      <c r="D2" s="23" t="n">
         <v>200</v>
       </c>
       <c r="E2" s="2" t="b">
@@ -4289,16 +4292,16 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="22" t="n">
+      <c r="C3" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="22" t="n">
+      <c r="D3" s="23" t="n">
         <v>200</v>
       </c>
       <c r="E3" s="2" t="b">
@@ -4311,16 +4314,16 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="22" t="n">
+      <c r="C4" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="22" t="n">
+      <c r="D4" s="23" t="n">
         <v>200</v>
       </c>
       <c r="E4" s="2" t="b">
@@ -4333,16 +4336,16 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="22" t="n">
+      <c r="D5" s="23" t="n">
         <v>200</v>
       </c>
       <c r="E5" s="2" t="b">
@@ -4355,16 +4358,16 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="22" t="n">
+      <c r="C6" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="22" t="n">
+      <c r="D6" s="23" t="n">
         <v>200</v>
       </c>
       <c r="E6" s="2" t="b">
@@ -4380,7 +4383,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -4402,7 +4405,7 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="24" t="s">
         <v>52</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -4424,7 +4427,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="24" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -4446,7 +4449,7 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="24" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -4468,7 +4471,7 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="24" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -4487,16 +4490,16 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="D12" s="14" t="n">
         <v>200</v>
       </c>
       <c r="E12" s="2" t="b">
@@ -4512,7 +4515,7 @@
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -4531,16 +4534,16 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="D14" s="14" t="n">
         <v>200</v>
       </c>
       <c r="E14" s="2" t="b">
@@ -4556,7 +4559,7 @@
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -4575,16 +4578,16 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="1" t="n">
+      <c r="C16" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="D16" s="14" t="n">
         <v>200</v>
       </c>
       <c r="E16" s="2" t="b">
@@ -4600,7 +4603,7 @@
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="1" t="n">
@@ -4619,16 +4622,16 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="1" t="n">
+      <c r="C18" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="D18" s="14" t="n">
         <v>200</v>
       </c>
       <c r="E18" s="2" t="b">
@@ -4644,7 +4647,7 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="1" t="n">
@@ -4663,16 +4666,16 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="1" t="n">
+      <c r="C20" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="D20" s="14" t="n">
         <v>200</v>
       </c>
       <c r="E20" s="2" t="b">
@@ -4703,8 +4706,8 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="1" sqref="D1:D2 F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4723,7 +4726,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="n">
+      <c r="A2" s="17" t="n">
         <v>45651</v>
       </c>
       <c r="B2" s="2" t="b">

</xml_diff>